<commit_message>
Updated the SIQ file PO1_DGC_SIQ_011
Signed-off-by: Hazemmekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Technical\ITI\Software Engineering\Tasks\Digital Calculator\SWE_Digital_Calculator\Input documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\Input documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169C203D-513A-4D76-A73F-6B6F58194AC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ" sheetId="3" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -177,11 +178,23 @@
   <si>
     <t>The GDD should only include application API's</t>
   </si>
+  <si>
+    <t>Hazem Mekawy</t>
+  </si>
+  <si>
+    <t>PO1_DGC_SIQ_011</t>
+  </si>
+  <si>
+    <t>Is there a clear switch ? And if there's one, should the clear switch be separate from the keypad ?</t>
+  </si>
+  <si>
+    <t>The switch shall be the '*' button in the keypad</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
@@ -535,14 +548,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1094,14 +1107,28 @@
       <c r="AA12" s="7"/>
     </row>
     <row r="13" spans="1:27" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="A13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="6">
+        <v>43885</v>
+      </c>
+      <c r="H13" s="10"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -29747,7 +29774,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="B2:C60">
+    <dataValidation type="list" allowBlank="1" sqref="B2:C60" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Hazem Mekawy,Esraa Awad,Nada Mohamed,Mina Helmi,Alzahraa El-Sallakh"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>